<commit_message>
Update contract + FE code
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LONG\nft-characters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E41525-DC42-4C99-9687-05B0986F6952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE751FD2-3993-4015-8134-2D15F5A5AB54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2085" windowWidth="21600" windowHeight="11385" activeTab="9" xr2:uid="{EAE5561F-10DE-4B28-A222-B4C0631CE220}"/>
+    <workbookView xWindow="2865" yWindow="2085" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{EAE5561F-10DE-4B28-A222-B4C0631CE220}"/>
   </bookViews>
   <sheets>
     <sheet name="back" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="267">
   <si>
     <t>Legendary</t>
   </si>
@@ -833,6 +833,39 @@
   </si>
   <si>
     <t>LEGENDARY</t>
+  </si>
+  <si>
+    <t>white green</t>
+  </si>
+  <si>
+    <t>yellow green</t>
+  </si>
+  <si>
+    <t>gradient blue</t>
+  </si>
+  <si>
+    <t>fire red</t>
+  </si>
+  <si>
+    <t>smooth green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sky </t>
+  </si>
+  <si>
+    <t>darkness</t>
+  </si>
+  <si>
+    <t>cutting edge</t>
+  </si>
+  <si>
+    <t>red tail</t>
+  </si>
+  <si>
+    <t>half blue</t>
+  </si>
+  <si>
+    <t>elizabeth sick</t>
   </si>
 </sst>
 </file>
@@ -911,10 +944,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1951,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54161073-895D-49B7-85B0-5591B6FC464A}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,7 +2146,7 @@
       </c>
       <c r="B7" s="2">
         <f>COUNT(fur!$C$2:$C$100)</f>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2">
         <f>COUNTIF(fur!$B$2:$B$100,$C$1)</f>
@@ -2121,11 +2154,11 @@
       </c>
       <c r="D7" s="2">
         <f>COUNTIF(fur!$B$2:$B$100,$D$1)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
         <f>COUNTIF(fur!$B$2:$B$100,$E$1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F7" s="2">
         <f>COUNTIF(fur!$B$2:$B$100,$F$1)</f>
@@ -2208,19 +2241,19 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2231,15 +2264,15 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2">
         <f ca="1">RANDBETWEEN(0,VALUE(C2) - 1)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2">
         <f ca="1">RANDBETWEEN(0,VALUE(D2) - 1)+40</f>
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2">
         <f ca="1">RANDBETWEEN(0,VALUE(E2)-1)+70</f>
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F13" s="2">
         <f ca="1">RANDBETWEEN(0,VALUE(F2) - 1)+90</f>
@@ -2248,11 +2281,11 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">TEXT(INDEX(C13:F13,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>02</v>
+        <v>70</v>
       </c>
       <c r="I13" t="str">
         <f ca="1">IF(VALUE(H13)= C13, "Common", IF(VALUE(H13) = D13, "Rare", IF(VALUE(H13) = E13, "Epic", "Legendary")))</f>
-        <v>Common</v>
+        <v>Epic</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>251</v>
@@ -2265,7 +2298,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C21" ca="1" si="0">RANDBETWEEN(0,VALUE(C3) - 1)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" ref="D14:D21" ca="1" si="1">RANDBETWEEN(0,VALUE(D3) - 1)+40</f>
@@ -2277,20 +2310,20 @@
       </c>
       <c r="F14" s="2">
         <f t="shared" ref="F14:F21" ca="1" si="3">RANDBETWEEN(0,VALUE(F3) - 1)+90</f>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">TEXT(INDEX(C14:F14,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>40</v>
+        <v>02</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ref="I14:I21" ca="1" si="4">IF(VALUE(H14)= C14, "Common", IF(VALUE(H14) = D14, "Rare", IF(VALUE(H14) = E14, "Epic", "Legendary")))</f>
-        <v>Rare</v>
+        <v>Common</v>
       </c>
       <c r="K14" t="str">
         <f ca="1">_xlfn.CONCAT($H$13:$H$21)</f>
-        <v>024043130101170350</v>
+        <v>700274754070094747</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2300,7 +2333,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2308,20 +2341,20 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">TEXT(INDEX(C15:F15,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Rare</v>
+        <v>Epic</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2331,28 +2364,28 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">TEXT(INDEX(C16:F16,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Common</v>
+        <v>Epic</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2362,7 +2395,7 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2370,20 +2403,20 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">TEXT(INDEX(C17:F17,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>01</v>
+        <v>40</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Common</v>
+        <v>Rare</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2393,15 +2426,15 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E18" s="2" t="e">
+        <v>40</v>
+      </c>
+      <c r="E18" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
+        <v>70</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ca="1" si="3"/>
@@ -2410,11 +2443,11 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">TEXT(INDEX(C18:F18,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>01</v>
+        <v>70</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Common</v>
+        <v>Epic</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2424,15 +2457,15 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ca="1" si="3"/>
@@ -2441,7 +2474,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">TEXT(INDEX(C19:F19,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>17</v>
+        <v>09</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2458,32 +2491,32 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">TEXT(INDEX(C20:F20,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>03</v>
+        <v>47</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Common</v>
+        <v>Rare</v>
       </c>
       <c r="K20" t="str">
         <f ca="1">_xlfn.CONCAT(F13:F21)</f>
-        <v>909091919290919592</v>
+        <v>909190909090919292</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2493,15 +2526,15 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" ca="1" si="3"/>
@@ -2510,7 +2543,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">TEXT(INDEX(C21:F21,,RANDBETWEEN(1,3),1), "00")</f>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3789,10 +3822,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598DB440-1FD3-40E2-943C-89C8311D050D}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3965,8 +3998,172 @@
         <v>105</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2">
+        <v>46</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="2">
+        <v>70</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2">
+        <v>71</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="2">
+        <v>72</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2">
+        <v>9</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B12">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3976,7 +4173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1">
+  <conditionalFormatting sqref="B13:B23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3994,7 +4191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DCC219-A4CA-4E05-A7DF-12B9BB4D7A80}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>